<commit_message>
added absolute sum to calculate error instead
</commit_message>
<xml_diff>
--- a/Plot/Final_Draft_Position_Graphs.xlsx
+++ b/Plot/Final_Draft_Position_Graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\PycharmProjects\MQP_Stat\Plot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Desktop\MQP\Plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85597FF3-65E3-46DB-933E-A18E8BEA1AAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AB8B72-E57C-475B-A8A8-0EDFD488CC94}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" tabRatio="881" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="881" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Draft Value Calculation Tool" sheetId="21" r:id="rId1"/>
@@ -28,6 +28,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="91">
   <si>
     <t>Draft Position</t>
   </si>
@@ -470,6 +471,12 @@
   </si>
   <si>
     <t>54 - 58,60</t>
+  </si>
+  <si>
+    <t>ABSSUM</t>
+  </si>
+  <si>
+    <t>Rk</t>
   </si>
 </sst>
 </file>
@@ -10247,7 +10254,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8656674" cy="6282070"/>
+    <xdr:ext cx="8656320" cy="6278880"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -11099,21 +11106,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E46C26E-3F42-42E6-AFD3-CAD7FBC5552A}">
-  <dimension ref="A1:Z62"/>
+  <dimension ref="A1:AA62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R4" workbookViewId="0">
-      <selection activeCell="Z19" sqref="Z19"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="94" workbookViewId="0">
+      <selection activeCell="AA29" sqref="AA29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="12" max="12" width="10.3125" customWidth="1"/>
-    <col min="13" max="13" width="11.68359375" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="11.6640625" customWidth="1"/>
     <col min="17" max="17" width="13" customWidth="1"/>
-    <col min="21" max="21" width="12.578125" customWidth="1"/>
+    <col min="21" max="21" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -11142,7 +11149,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -11172,7 +11179,7 @@
         <v>0.99999999597030709</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -11202,7 +11209,7 @@
         <v>0.90282866147944207</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -11232,7 +11239,7 @@
         <v>0.83652025761259374</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -11280,7 +11287,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -11331,7 +11338,7 @@
         <v>5.989132618275083E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -11382,7 +11389,7 @@
         <v>2.0262447580083134E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -11433,7 +11440,7 @@
         <v>-1.2433483748086869E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -11478,7 +11485,7 @@
         <v>-0.10111030285964551</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -11523,7 +11530,7 @@
         <v>-0.10681174272108007</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -11570,7 +11577,7 @@
         <v>4.0280257324320362E-4</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -11615,7 +11622,7 @@
         <v>-1.8366442392827191E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -11657,7 +11664,7 @@
         <v>-2.2595056483651801E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -11696,7 +11703,7 @@
       </c>
       <c r="Q14" s="6"/>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -11735,7 +11742,7 @@
       </c>
       <c r="Q15" s="6"/>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -11765,7 +11772,7 @@
         <v>0.44960492615641728</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -11795,7 +11802,7 @@
         <v>0.42946305153273773</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -11828,7 +11835,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -11891,7 +11898,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -11964,7 +11971,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -12037,7 +12044,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -12110,7 +12117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -12183,7 +12190,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -12256,7 +12263,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -12329,7 +12336,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -12402,7 +12409,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -12475,7 +12482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -12504,8 +12511,17 @@
         <f t="shared" si="0"/>
         <v>0.26239919945626994</v>
       </c>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="Y28" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>89</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -12534,8 +12550,66 @@
         <f t="shared" si="0"/>
         <v>0.25101159526234518</v>
       </c>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="M29" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="N29">
+        <f>ABS(N20)</f>
+        <v>0.28821519434524068</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ref="O29:Y29" si="2">ABS(O20)</f>
+        <v>0.31372909919083436</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="2"/>
+        <v>0.15420658316733421</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" si="2"/>
+        <v>0.138785232156446</v>
+      </c>
+      <c r="R29">
+        <f t="shared" si="2"/>
+        <v>3.7625167359855854E-2</v>
+      </c>
+      <c r="S29">
+        <f t="shared" si="2"/>
+        <v>0.10045450632182384</v>
+      </c>
+      <c r="T29">
+        <f t="shared" si="2"/>
+        <v>0.24159094035210615</v>
+      </c>
+      <c r="U29">
+        <f t="shared" si="2"/>
+        <v>0.16489386441204612</v>
+      </c>
+      <c r="V29">
+        <f t="shared" si="2"/>
+        <v>0.10911318325619712</v>
+      </c>
+      <c r="W29">
+        <f t="shared" si="2"/>
+        <v>3.4303204106291188E-2</v>
+      </c>
+      <c r="X29">
+        <f t="shared" si="2"/>
+        <v>5.989132618275083E-2</v>
+      </c>
+      <c r="Y29">
+        <f>AVERAGE(N29:X29)</f>
+        <v>0.14934620916826602</v>
+      </c>
+      <c r="Z29">
+        <f>SUM(N29:X29)</f>
+        <v>1.6428083008509262</v>
+      </c>
+      <c r="AA29">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -12564,8 +12638,66 @@
         <f t="shared" si="0"/>
         <v>0.24011385822110282</v>
       </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="M30" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="N30">
+        <f t="shared" ref="N30:Y30" si="3">ABS(N21)</f>
+        <v>0.1442109548140984</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="3"/>
+        <v>0.16755691149508284</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="3"/>
+        <v>6.953039473692621E-2</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" si="3"/>
+        <v>5.7145325751564724E-2</v>
+      </c>
+      <c r="R30">
+        <f t="shared" si="3"/>
+        <v>3.2012951929989708E-3</v>
+      </c>
+      <c r="S30">
+        <f t="shared" si="3"/>
+        <v>5.0325894244425184E-2</v>
+      </c>
+      <c r="T30">
+        <f t="shared" si="3"/>
+        <v>0.13374857622133329</v>
+      </c>
+      <c r="U30">
+        <f t="shared" si="3"/>
+        <v>8.0616389683198175E-2</v>
+      </c>
+      <c r="V30">
+        <f t="shared" si="3"/>
+        <v>3.9191642515022301E-2</v>
+      </c>
+      <c r="W30">
+        <f t="shared" si="3"/>
+        <v>1.1481914487998224E-2</v>
+      </c>
+      <c r="X30">
+        <f t="shared" si="3"/>
+        <v>2.0262447580083134E-2</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" ref="Y30:Y36" si="4">AVERAGE(N30:X30)</f>
+        <v>7.0661067883884654E-2</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" ref="Z30:Z36" si="5">SUM(N30:X30)</f>
+        <v>0.77727174672273125</v>
+      </c>
+      <c r="AA30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -12594,8 +12726,66 @@
         <f t="shared" si="0"/>
         <v>0.22967998875887949</v>
       </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+      <c r="M31" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="N31">
+        <f t="shared" ref="N31:Y31" si="6">ABS(N22)</f>
+        <v>9.5654216032531769E-2</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="6"/>
+        <v>0.12675678011361802</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="6"/>
+        <v>4.4172297185029019E-2</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" si="6"/>
+        <v>3.4772917119035129E-2</v>
+      </c>
+      <c r="R31">
+        <f t="shared" si="6"/>
+        <v>9.5624380165017231E-3</v>
+      </c>
+      <c r="S31">
+        <f t="shared" si="6"/>
+        <v>1.0208526066898149E-2</v>
+      </c>
+      <c r="T31">
+        <f t="shared" si="6"/>
+        <v>9.7837274310697386E-2</v>
+      </c>
+      <c r="U31">
+        <f t="shared" si="6"/>
+        <v>3.2056267090288415E-2</v>
+      </c>
+      <c r="V31">
+        <f t="shared" si="6"/>
+        <v>2.0761704604279396E-2</v>
+      </c>
+      <c r="W31">
+        <f t="shared" si="6"/>
+        <v>1.566653194181045E-2</v>
+      </c>
+      <c r="X31">
+        <f t="shared" si="6"/>
+        <v>1.2433483748086869E-2</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" si="4"/>
+        <v>4.5443857838979668E-2</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" si="5"/>
+        <v>0.49988243622877637</v>
+      </c>
+      <c r="AA31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -12624,8 +12814,66 @@
         <f t="shared" si="0"/>
         <v>0.21968532284116465</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="M32" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N32">
+        <f t="shared" ref="N32:Y32" si="7">ABS(N23)</f>
+        <v>0.29020790313497269</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="7"/>
+        <v>0.31568151242099995</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="7"/>
+        <v>0.1738803109943059</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" si="7"/>
+        <v>0.16129896439521973</v>
+      </c>
+      <c r="R32">
+        <f t="shared" si="7"/>
+        <v>0.11983761967336265</v>
+      </c>
+      <c r="S32">
+        <f t="shared" si="7"/>
+        <v>1.2771024967148326E-2</v>
+      </c>
+      <c r="T32">
+        <f t="shared" si="7"/>
+        <v>0.24315789062011151</v>
+      </c>
+      <c r="U32">
+        <f t="shared" si="7"/>
+        <v>0.16922830235905123</v>
+      </c>
+      <c r="V32">
+        <f t="shared" si="7"/>
+        <v>0.14354741568112156</v>
+      </c>
+      <c r="W32">
+        <f t="shared" si="7"/>
+        <v>0.10968884925849437</v>
+      </c>
+      <c r="X32">
+        <f t="shared" si="7"/>
+        <v>0.10111030285964551</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" si="4"/>
+        <v>0.16731000876040306</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" si="5"/>
+        <v>1.8404100963644336</v>
+      </c>
+      <c r="AA32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -12654,8 +12902,66 @@
         <f t="shared" si="0"/>
         <v>0.21010639021975655</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="M33" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="N33">
+        <f t="shared" ref="N33:Y33" si="8">ABS(N24)</f>
+        <v>0.40683585508469478</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="8"/>
+        <v>0.42959792633672933</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="8"/>
+        <v>0.1841280366507928</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" si="8"/>
+        <v>0.16057628549038516</v>
+      </c>
+      <c r="R33">
+        <f t="shared" si="8"/>
+        <v>9.6226415094339712E-2</v>
+      </c>
+      <c r="S33">
+        <f t="shared" si="8"/>
+        <v>4.865272168304291E-2</v>
+      </c>
+      <c r="T33">
+        <f t="shared" si="8"/>
+        <v>0.30042196636325269</v>
+      </c>
+      <c r="U33">
+        <f t="shared" si="8"/>
+        <v>0.20535294472240639</v>
+      </c>
+      <c r="V33">
+        <f t="shared" si="8"/>
+        <v>0.13477002833202717</v>
+      </c>
+      <c r="W33">
+        <f t="shared" si="8"/>
+        <v>0.11180903008017332</v>
+      </c>
+      <c r="X33">
+        <f t="shared" si="8"/>
+        <v>0.10681174272108007</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" si="4"/>
+        <v>0.19865299568717495</v>
+      </c>
+      <c r="Z33">
+        <f t="shared" si="5"/>
+        <v>2.1851829525589244</v>
+      </c>
+      <c r="AA33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -12684,8 +12990,66 @@
         <f t="shared" si="0"/>
         <v>0.20092079185928943</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="M34" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="N34">
+        <f t="shared" ref="N34:Y34" si="9">ABS(N25)</f>
+        <v>0.16086908692358221</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="9"/>
+        <v>0.18376060914691444</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="9"/>
+        <v>8.7642201256913438E-2</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" si="9"/>
+        <v>7.5498210509820807E-2</v>
+      </c>
+      <c r="R34">
+        <f t="shared" si="9"/>
+        <v>2.2604213008604379E-2</v>
+      </c>
+      <c r="S34">
+        <f t="shared" si="9"/>
+        <v>4.9346289049000625E-2</v>
+      </c>
+      <c r="T34">
+        <f t="shared" si="9"/>
+        <v>0.15061036095497504</v>
+      </c>
+      <c r="U34">
+        <f t="shared" si="9"/>
+        <v>9.8512404742171711E-2</v>
+      </c>
+      <c r="V34">
+        <f t="shared" si="9"/>
+        <v>5.7893999878575936E-2</v>
+      </c>
+      <c r="W34">
+        <f t="shared" si="9"/>
+        <v>8.2068154071532756E-3</v>
+      </c>
+      <c r="X34">
+        <f t="shared" si="9"/>
+        <v>4.0280257324320362E-4</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" si="4"/>
+        <v>8.1395181222814098E-2</v>
+      </c>
+      <c r="Z34">
+        <f t="shared" si="5"/>
+        <v>0.89534699345095514</v>
+      </c>
+      <c r="AA34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -12714,8 +13078,66 @@
         <f t="shared" si="0"/>
         <v>0.1921070933293563</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="M35" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="N35">
+        <f t="shared" ref="N35:Y35" si="10">ABS(N26)</f>
+        <v>0.17661259906251447</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="10"/>
+        <v>0.19907463769468625</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="10"/>
+        <v>0.10475957335669842</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" si="10"/>
+        <v>9.2843424371555544E-2</v>
+      </c>
+      <c r="R35">
+        <f t="shared" si="10"/>
+        <v>4.0941807533189462E-2</v>
+      </c>
+      <c r="S35">
+        <f t="shared" si="10"/>
+        <v>4.8420469384216902E-2</v>
+      </c>
+      <c r="T35">
+        <f t="shared" si="10"/>
+        <v>0.16654634410683256</v>
+      </c>
+      <c r="U35">
+        <f t="shared" si="10"/>
+        <v>0.11542583347882224</v>
+      </c>
+      <c r="V35">
+        <f t="shared" si="10"/>
+        <v>7.5569498442554756E-2</v>
+      </c>
+      <c r="W35">
+        <f t="shared" si="10"/>
+        <v>2.6814529409373268E-2</v>
+      </c>
+      <c r="X35">
+        <f t="shared" si="10"/>
+        <v>1.8366442392827191E-2</v>
+      </c>
+      <c r="Y35">
+        <f t="shared" si="4"/>
+        <v>9.6852287203024634E-2</v>
+      </c>
+      <c r="Z35">
+        <f t="shared" si="5"/>
+        <v>1.065375159233271</v>
+      </c>
+      <c r="AA35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -12744,8 +13166,66 @@
         <f t="shared" si="0"/>
         <v>0.18364473158317046</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="M36" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="N36">
+        <f t="shared" ref="N36:Y36" si="11">ABS(N27)</f>
+        <v>0.22322940134251934</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="11"/>
+        <v>0.24802249662840925</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="11"/>
+        <v>0.1169027710497143</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" si="11"/>
+        <v>0.10298862282771812</v>
+      </c>
+      <c r="R36">
+        <f t="shared" si="11"/>
+        <v>4.7142707982693238E-2</v>
+      </c>
+      <c r="S36">
+        <f t="shared" si="11"/>
+        <v>4.2823197083251441E-2</v>
+      </c>
+      <c r="T36">
+        <f t="shared" si="11"/>
+        <v>0.19055905041847271</v>
+      </c>
+      <c r="U36">
+        <f t="shared" si="11"/>
+        <v>0.12372657235542639</v>
+      </c>
+      <c r="V36">
+        <f t="shared" si="11"/>
+        <v>8.2978210387111173E-2</v>
+      </c>
+      <c r="W36">
+        <f t="shared" si="11"/>
+        <v>3.2342948214673622E-2</v>
+      </c>
+      <c r="X36">
+        <f t="shared" si="11"/>
+        <v>2.2595056483651801E-2</v>
+      </c>
+      <c r="Y36">
+        <f t="shared" si="4"/>
+        <v>0.11211918497942196</v>
+      </c>
+      <c r="Z36">
+        <f t="shared" si="5"/>
+        <v>1.2333110347736416</v>
+      </c>
+      <c r="AA36">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -12775,7 +13255,7 @@
         <v>0.17551393303665236</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -12805,7 +13285,7 @@
         <v>0.16769564124788411</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -12835,7 +13315,7 @@
         <v>0.16017145280161332</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -12865,7 +13345,7 @@
         <v>0.15292356024586137</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -12895,7 +13375,7 @@
         <v>0.14593470112183102</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -12925,7 +13405,7 @@
         <v>0.1391881122848814</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -12955,7 +13435,7 @@
         <v>0.13266748884143445</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -12985,7 +13465,7 @@
         <v>0.12635694713048187</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -13015,7 +13495,7 @@
         <v>0.12024099126365417</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -13045,7 +13525,7 @@
         <v>0.11430448280829171</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -13075,7 +13555,7 @@
         <v>0.1085326132565151</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -13105,7 +13585,7 @@
         <v>0.10291087897219527</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -13135,7 +13615,7 @@
         <v>9.7425058348779014E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -13165,7 +13645,7 @@
         <v>9.2061190945554844E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -13195,7 +13675,7 @@
         <v>8.6805558399283569E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -13225,7 +13705,7 @@
         <v>8.1644666933101392E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -13255,7 +13735,7 @@
         <v>7.6565231305956119E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -13285,7 +13765,7 @@
         <v>7.1554160064165415E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -13315,7 +13795,7 @@
         <v>6.6598541972489822E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -13345,7 +13825,7 @@
         <v>6.168563351577934E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -13375,7 +13855,7 @@
         <v>5.6802847374120689E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -13405,7 +13885,7 @@
         <v>5.1937741784757512E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -13435,7 +13915,7 @@
         <v>4.7078010713098549E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -13465,7 +13945,7 @@
         <v>4.2211474763059698E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -13495,7 +13975,7 @@
         <v>3.7326072763972151E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B62">
         <v>0</v>
       </c>
@@ -13567,21 +14047,21 @@
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="14.7890625" customWidth="1"/>
-    <col min="2" max="2" width="36.68359375" customWidth="1"/>
-    <col min="3" max="4" width="24.5234375" customWidth="1"/>
-    <col min="5" max="6" width="29.7890625" customWidth="1"/>
-    <col min="7" max="8" width="27.5234375" customWidth="1"/>
-    <col min="9" max="10" width="34.41796875" customWidth="1"/>
-    <col min="11" max="12" width="40.89453125" customWidth="1"/>
-    <col min="13" max="13" width="35.3125" customWidth="1"/>
-    <col min="14" max="14" width="33.5234375" customWidth="1"/>
-    <col min="15" max="15" width="12.89453125" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="4" width="24.5546875" customWidth="1"/>
+    <col min="5" max="6" width="29.77734375" customWidth="1"/>
+    <col min="7" max="8" width="27.5546875" customWidth="1"/>
+    <col min="9" max="10" width="34.44140625" customWidth="1"/>
+    <col min="11" max="12" width="40.88671875" customWidth="1"/>
+    <col min="13" max="13" width="35.33203125" customWidth="1"/>
+    <col min="14" max="14" width="33.5546875" customWidth="1"/>
+    <col min="15" max="15" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -13628,7 +14108,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -13681,7 +14161,7 @@
         <v>6975366.666666667</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -13734,7 +14214,7 @@
         <v>6241066.666666667</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -13787,7 +14267,7 @@
         <v>5604500</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -13840,7 +14320,7 @@
         <v>5053066.666666667</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -13893,7 +14373,7 @@
         <v>4575800</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -13946,7 +14426,7 @@
         <v>4156066.6666666665</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -13999,7 +14479,7 @@
         <v>3793933.3333333335</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -14052,7 +14532,7 @@
         <v>3475733.3333333335</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -14105,7 +14585,7 @@
         <v>3194966.6666666665</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -14158,7 +14638,7 @@
         <v>3035100</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -14211,7 +14691,7 @@
         <v>2883433.3333333335</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -14264,7 +14744,7 @@
         <v>2739366.6666666665</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -14317,7 +14797,7 @@
         <v>2602366.6666666665</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -14370,7 +14850,7 @@
         <v>2472300</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -14423,7 +14903,7 @@
         <v>2348433.3333333335</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -14476,7 +14956,7 @@
         <v>2231200</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -14529,7 +15009,7 @@
         <v>2119566.6666666665</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -14582,7 +15062,7 @@
         <v>2013666.6666666667</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -14635,7 +15115,7 @@
         <v>1922933.3333333333</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -14688,7 +15168,7 @@
         <v>1845900</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -14741,7 +15221,7 @@
         <v>1772133.3333333333</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -14794,7 +15274,7 @@
         <v>1701300</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -14847,7 +15327,7 @@
         <v>1633266.6666666667</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -14900,7 +15380,7 @@
         <v>1568000</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -14953,7 +15433,7 @@
         <v>1505233.3333333333</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -15006,7 +15486,7 @@
         <v>1455300</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -15059,7 +15539,7 @@
         <v>1413333.3333333333</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -15112,7 +15592,7 @@
         <v>1404666.6666666667</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -15165,7 +15645,7 @@
         <v>1394400</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -15218,7 +15698,7 @@
         <v>1384400</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -15271,7 +15751,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -15324,7 +15804,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -15377,7 +15857,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -15430,7 +15910,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -15483,7 +15963,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -15536,7 +16016,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -15589,7 +16069,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -15642,7 +16122,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -15695,7 +16175,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -15748,7 +16228,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -15801,7 +16281,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -15854,7 +16334,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -15907,7 +16387,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -15960,7 +16440,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -16013,7 +16493,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -16066,7 +16546,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -16119,7 +16599,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -16172,7 +16652,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -16225,7 +16705,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -16278,7 +16758,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -16331,7 +16811,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -16384,7 +16864,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -16437,7 +16917,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -16490,7 +16970,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -16543,7 +17023,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -16596,7 +17076,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -16649,7 +17129,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="59" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -16702,7 +17182,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="60" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -16755,7 +17235,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="61" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -16821,20 +17301,20 @@
       <selection activeCell="A17" sqref="A17:I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.41796875" customWidth="1"/>
-    <col min="2" max="2" width="29.5234375" customWidth="1"/>
-    <col min="3" max="3" width="19.7890625" customWidth="1"/>
-    <col min="4" max="4" width="20.20703125" customWidth="1"/>
-    <col min="5" max="5" width="20.7890625" customWidth="1"/>
-    <col min="6" max="6" width="28.1015625" customWidth="1"/>
-    <col min="7" max="7" width="33.68359375" customWidth="1"/>
-    <col min="8" max="8" width="35.3125" customWidth="1"/>
-    <col min="9" max="9" width="18.3125" customWidth="1"/>
+    <col min="1" max="1" width="19.44140625" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.77734375" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" customWidth="1"/>
+    <col min="5" max="5" width="20.77734375" customWidth="1"/>
+    <col min="6" max="6" width="28.109375" customWidth="1"/>
+    <col min="7" max="7" width="33.6640625" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" customWidth="1"/>
+    <col min="9" max="9" width="18.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -16863,7 +17343,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -16900,7 +17380,7 @@
         <v>18820933.333333336</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -16937,7 +17417,7 @@
         <v>17578866.666666668</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -16974,7 +17454,7 @@
         <v>20403266.666666668</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -17011,7 +17491,7 @@
         <v>27713733.333333332</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
@@ -17048,7 +17528,7 @@
         <v>12846870</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -17085,7 +17565,7 @@
         <v>12846870</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>26</v>
       </c>
@@ -17111,7 +17591,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>2</v>
       </c>
@@ -17148,7 +17628,7 @@
         <v>6273644.444444445</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>5.5</v>
       </c>
@@ -17185,7 +17665,7 @@
         <v>4394716.666666667</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -17222,7 +17702,7 @@
         <v>2914752.3809523811</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>22.5</v>
       </c>
@@ -17259,7 +17739,7 @@
         <v>1732108.3333333333</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>38</v>
       </c>
@@ -17296,7 +17776,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>53</v>
       </c>
@@ -17333,7 +17813,7 @@
         <v>856458</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>26</v>
       </c>
@@ -17362,7 +17842,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>2</v>
       </c>
@@ -17398,7 +17878,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>5.5</v>
       </c>
@@ -17434,7 +17914,7 @@
         <v>70.050458000665927</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>11</v>
       </c>
@@ -17470,7 +17950,7 @@
         <v>46.460273717512109</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>22.5</v>
       </c>
@@ -17506,7 +17986,7 @@
         <v>27.60928434296563</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>38</v>
       </c>
@@ -17542,7 +18022,7 @@
         <v>13.65168216949921</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>53</v>
       </c>
@@ -17578,7 +18058,7 @@
         <v>13.65168216949921</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C25" t="s">
         <v>36</v>
       </c>
@@ -17598,7 +18078,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C26">
         <f>C10/I10</f>
         <v>9.6634952570542009E-4</v>
@@ -17624,7 +18104,7 @@
         <v>0.11409193646082021</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C27">
         <f t="shared" ref="C27:C30" si="11">C11/I11</f>
         <v>1.079136690647482E-3</v>
@@ -17650,7 +18130,7 @@
         <v>0.11909999829340531</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C28">
         <f t="shared" si="11"/>
         <v>1.3586353819159676E-3</v>
@@ -17676,7 +18156,7 @@
         <v>0.13394798659691748</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C29">
         <f t="shared" si="11"/>
         <v>1.4756402361284177E-3</v>
@@ -17702,7 +18182,7 @@
         <v>0.12544675371536618</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C30">
         <f t="shared" si="11"/>
         <v>1.4629166481796736E-3</v>
@@ -17728,7 +18208,7 @@
         <v>0.10234940183873581</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C31">
         <f>C15/I15</f>
         <v>7.5479085567145934E-4</v>
@@ -17754,7 +18234,7 @@
         <v>5.0692237097440862E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B32" s="3" t="s">
         <v>26</v>
       </c>
@@ -17777,7 +18257,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="33" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B33" s="2">
         <v>2</v>
       </c>
@@ -17800,7 +18280,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B34" s="2">
         <v>5.5</v>
       </c>
@@ -17829,7 +18309,7 @@
         <v>104.38949716253856</v>
       </c>
     </row>
-    <row r="35" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B35" s="2">
         <v>11</v>
       </c>
@@ -17858,7 +18338,7 @@
         <v>117.40355304069648</v>
       </c>
     </row>
-    <row r="36" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B36" s="3">
         <v>22.5</v>
       </c>
@@ -17887,7 +18367,7 @@
         <v>109.9523402910493</v>
       </c>
     </row>
-    <row r="37" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B37" s="3">
         <v>38</v>
       </c>
@@ -17916,7 +18396,7 @@
         <v>89.707831619875222</v>
       </c>
     </row>
-    <row r="38" spans="2:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="2:8" x14ac:dyDescent="0.3">
       <c r="B38" s="3">
         <v>53</v>
       </c>
@@ -17958,19 +18438,19 @@
       <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.3125" customWidth="1"/>
-    <col min="2" max="2" width="34.68359375" customWidth="1"/>
-    <col min="3" max="3" width="20.3125" customWidth="1"/>
-    <col min="4" max="4" width="14.3125" customWidth="1"/>
-    <col min="5" max="5" width="30.5234375" customWidth="1"/>
-    <col min="6" max="6" width="22.1015625" customWidth="1"/>
-    <col min="7" max="7" width="19.41796875" customWidth="1"/>
-    <col min="8" max="8" width="20.20703125" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="2" max="2" width="34.6640625" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" customWidth="1"/>
+    <col min="6" max="6" width="22.109375" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
+    <col min="8" max="8" width="20.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>48</v>
       </c>
@@ -17996,7 +18476,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -18022,7 +18502,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5.5</v>
       </c>
@@ -18048,7 +18528,7 @@
         <v>70.050458000665927</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>11</v>
       </c>
@@ -18074,7 +18554,7 @@
         <v>46.460273717512109</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>22.5</v>
       </c>
@@ -18100,7 +18580,7 @@
         <v>27.60928434296563</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>38</v>
       </c>
@@ -18126,7 +18606,7 @@
         <v>13.65168216949921</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>53</v>
       </c>
@@ -18152,12 +18632,12 @@
         <v>13.65168216949921</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="16.5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:8" ht="16.2" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>54</v>
       </c>
@@ -18180,7 +18660,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>57</v>
       </c>
@@ -18206,7 +18686,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>1</v>
       </c>
@@ -18239,7 +18719,7 @@
         <v>116.48</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
@@ -18272,7 +18752,7 @@
         <v>97.383795175573511</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>3</v>
       </c>
@@ -18305,7 +18785,7 @@
         <v>86.213231447193579</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>4</v>
       </c>
@@ -18338,7 +18818,7 @@
         <v>78.287590351147017</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>5</v>
       </c>
@@ -18371,7 +18851,7 @@
         <v>72.139985512440546</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>6</v>
       </c>
@@ -18404,7 +18884,7 @@
         <v>67.117026622767085</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>7</v>
       </c>
@@ -18437,7 +18917,7 @@
         <v>62.870175393526125</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>8</v>
       </c>
@@ -18470,7 +18950,7 @@
         <v>59.191385526720531</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>9</v>
       </c>
@@ -18503,7 +18983,7 @@
         <v>55.946462894387153</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>10</v>
       </c>
@@ -18536,7 +19016,7 @@
         <v>53.043780688014039</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>11</v>
       </c>
@@ -18569,7 +19049,7 @@
         <v>50.417985234404895</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>12</v>
       </c>
@@ -18602,7 +19082,7 @@
         <v>48.020821798340592</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>13</v>
       </c>
@@ -18635,7 +19115,7 @@
         <v>45.815645201934672</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>14</v>
       </c>
@@ -18668,7 +19148,7 @@
         <v>43.773970569099632</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>15</v>
       </c>
@@ -18701,7 +19181,7 @@
         <v>41.873216959634121</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>16</v>
       </c>
@@ -18734,7 +19214,7 @@
         <v>40.09518070229403</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>17</v>
       </c>
@@ -18767,7 +19247,7 @@
         <v>38.424972371251243</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>18</v>
       </c>
@@ -18800,7 +19280,7 @@
         <v>36.850258069960674</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>19</v>
       </c>
@@ -18833,7 +19313,7 @@
         <v>35.360706123964576</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>20</v>
       </c>
@@ -18866,7 +19346,7 @@
         <v>33.947575863587559</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>21</v>
       </c>
@@ -18899,7 +19379,7 @@
         <v>32.6034068407197</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>22</v>
       </c>
@@ -18932,7 +19412,7 @@
         <v>31.321780409978388</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>23</v>
       </c>
@@ -18965,7 +19445,7 @@
         <v>30.097134351151922</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>24</v>
       </c>
@@ -18998,7 +19478,7 @@
         <v>28.924616973914098</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>25</v>
       </c>
@@ -19031,7 +19511,7 @@
         <v>27.799971024881074</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>26</v>
       </c>
@@ -19064,7 +19544,7 @@
         <v>26.719440377508164</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>27</v>
       </c>
@@ -19097,7 +19577,7 @@
         <v>25.679694341580728</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>28</v>
       </c>
@@ -19130,7 +19610,7 @@
         <v>24.677765744673138</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>29</v>
       </c>
@@ -19163,7 +19643,7 @@
         <v>23.710999883872645</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>30</v>
       </c>
@@ -19196,7 +19676,7 @@
         <v>22.777012135207613</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>31</v>
       </c>
@@ -19229,7 +19709,7 @@
         <v>21.87365251643422</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>32</v>
       </c>
@@ -19262,7 +19742,7 @@
         <v>20.998975877867537</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>33</v>
       </c>
@@ -19295,7 +19775,7 @@
         <v>20.15121668159847</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>34</v>
       </c>
@@ -19328,7 +19808,7 @@
         <v>19.32876754682475</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>35</v>
       </c>
@@ -19361,7 +19841,7 @@
         <v>18.530160905966653</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>36</v>
       </c>
@@ -19394,7 +19874,7 @@
         <v>17.754053245534166</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>37</v>
       </c>
@@ -19427,7 +19907,7 @@
         <v>16.999211506651619</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>38</v>
       </c>
@@ -19460,7 +19940,7 @@
         <v>16.264501299538082</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>39</v>
       </c>
@@ -19493,7 +19973,7 @@
         <v>15.548876649128246</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>40</v>
       </c>
@@ -19526,7 +20006,7 @@
         <v>14.851371039161052</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>41</v>
       </c>
@@ -19559,7 +20039,7 @@
         <v>14.171089562296316</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>42</v>
       </c>
@@ -19592,7 +20072,7 @@
         <v>13.507202016293206</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>43</v>
       </c>
@@ -19625,7 +20105,7 @@
         <v>12.858936812642355</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>44</v>
       </c>
@@ -19658,7 +20138,7 @@
         <v>12.225575585551908</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>45</v>
       </c>
@@ -19691,7 +20171,7 @@
         <v>11.606448406827695</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>46</v>
       </c>
@@ -19724,7 +20204,7 @@
         <v>11.000929526725429</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>47</v>
       </c>
@@ -19757,7 +20237,7 @@
         <v>10.408433572887887</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>48</v>
       </c>
@@ -19790,7 +20270,7 @@
         <v>9.8284121494876047</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>49</v>
       </c>
@@ -19823,7 +20303,7 @@
         <v>9.2603507870522463</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>50</v>
       </c>
@@ -19856,7 +20336,7 @@
         <v>8.7037662004545808</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>51</v>
       </c>
@@ -19889,7 +20369,7 @@
         <v>8.1582038184448322</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>52</v>
       </c>
@@ -19922,7 +20402,7 @@
         <v>7.6232355530816704</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>53</v>
       </c>
@@ -19955,7 +20435,7 @@
         <v>7.0984577816390413</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>54</v>
       </c>
@@ -19988,7 +20468,7 @@
         <v>6.5834895171542342</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>55</v>
       </c>
@@ -20021,7 +20501,7 @@
         <v>6.0779707468454234</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>56</v>
       </c>
@@ -20054,7 +20534,7 @@
         <v>5.5815609202466305</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>57</v>
       </c>
@@ -20087,7 +20567,7 @@
         <v>5.0939375711581363</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>58</v>
       </c>
@@ -20120,7 +20600,7 @@
         <v>4.614795059446152</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>59</v>
       </c>
@@ -20153,7 +20633,7 @@
         <v>4.1438434203974168</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>60</v>
       </c>
@@ -20199,9 +20679,9 @@
       <selection activeCell="R2" sqref="R2:R61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -20254,7 +20734,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -20322,7 +20802,7 @@
         <v>0.99999999597030709</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -20390,7 +20870,7 @@
         <v>0.90282866147944207</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -20458,7 +20938,7 @@
         <v>0.83652025761259374</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -20526,7 +21006,7 @@
         <v>0.78346636979597473</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -20594,7 +21074,7 @@
         <v>0.73811655924221764</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -20662,7 +21142,7 @@
         <v>0.69797436021466841</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -20730,7 +21210,7 @@
         <v>0.66168915696573805</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -20798,7 +21278,7 @@
         <v>0.62843950474000532</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -20866,7 +21346,7 @@
         <v>0.59768301613943531</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -20934,7 +21414,7 @@
         <v>0.56903887584250845</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -21002,7 +21482,7 @@
         <v>0.54222659514044824</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -21070,7 +21550,7 @@
         <v>0.51703148224635098</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -21138,7 +21618,7 @@
         <v>0.49328394227574429</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -21206,7 +21686,7 @@
         <v>0.47084643704199852</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -21274,7 +21754,7 @@
         <v>0.44960492615641728</v>
       </c>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -21342,7 +21822,7 @@
         <v>0.42946305153273773</v>
       </c>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -21410,7 +21890,7 @@
         <v>0.41033806689194446</v>
       </c>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -21478,7 +21958,7 @@
         <v>0.39215791420302598</v>
       </c>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -21546,7 +22026,7 @@
         <v>0.37485907572584598</v>
       </c>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -21614,7 +22094,7 @@
         <v>0.35838496380678037</v>
       </c>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -21682,7 +22162,7 @@
         <v>0.34268469186014894</v>
       </c>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -21750,7 +22230,7 @@
         <v>0.32771212095142838</v>
       </c>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -21818,7 +22298,7 @@
         <v>0.31342510922662575</v>
       </c>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -21886,7 +22366,7 @@
         <v>0.29978491307164773</v>
       </c>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -21954,7 +22434,7 @@
         <v>0.28675570345299156</v>
       </c>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -22022,7 +22502,7 @@
         <v>0.274304170886219</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -22090,7 +22570,7 @@
         <v>0.26239919945626994</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -22158,7 +22638,7 @@
         <v>0.25101159526234518</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -22226,7 +22706,7 @@
         <v>0.24011385822110282</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -22294,7 +22774,7 @@
         <v>0.22967998875887949</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -22362,7 +22842,7 @@
         <v>0.21968532284116465</v>
       </c>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -22430,7 +22910,7 @@
         <v>0.21010639021975655</v>
       </c>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -22498,7 +22978,7 @@
         <v>0.20092079185928943</v>
       </c>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -22566,7 +23046,7 @@
         <v>0.1921070933293563</v>
       </c>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -22634,7 +23114,7 @@
         <v>0.18364473158317046</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -22702,7 +23182,7 @@
         <v>0.17551393303665236</v>
       </c>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -22770,7 +23250,7 @@
         <v>0.16769564124788411</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -22838,7 +23318,7 @@
         <v>0.16017145280161332</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -22906,7 +23386,7 @@
         <v>0.15292356024586137</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -22974,7 +23454,7 @@
         <v>0.14593470112183102</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -23042,7 +23522,7 @@
         <v>0.1391881122848814</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -23110,7 +23590,7 @@
         <v>0.13266748884143445</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -23178,7 +23658,7 @@
         <v>0.12635694713048187</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -23246,7 +23726,7 @@
         <v>0.12024099126365417</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -23314,7 +23794,7 @@
         <v>0.11430448280829171</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -23382,7 +23862,7 @@
         <v>0.1085326132565151</v>
       </c>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -23450,7 +23930,7 @@
         <v>0.10291087897219527</v>
       </c>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -23518,7 +23998,7 @@
         <v>9.7425058348779014E-2</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -23586,7 +24066,7 @@
         <v>9.2061190945554844E-2</v>
       </c>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -23654,7 +24134,7 @@
         <v>8.6805558399283569E-2</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -23722,7 +24202,7 @@
         <v>8.1644666933101392E-2</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -23790,7 +24270,7 @@
         <v>7.6565231305956119E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -23858,7 +24338,7 @@
         <v>7.1554160064165415E-2</v>
       </c>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -23926,7 +24406,7 @@
         <v>6.6598541972489822E-2</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -23994,7 +24474,7 @@
         <v>6.168563351577934E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -24062,7 +24542,7 @@
         <v>5.6802847374120689E-2</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -24130,7 +24610,7 @@
         <v>5.1937741784757512E-2</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -24198,7 +24678,7 @@
         <v>4.7078010713098549E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -24266,7 +24746,7 @@
         <v>4.2211474763059698E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>

</xml_diff>

<commit_message>
added graphs, added to report
</commit_message>
<xml_diff>
--- a/Plot/Final_Draft_Position_Graphs.xlsx
+++ b/Plot/Final_Draft_Position_Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Desktop\MQP\Plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05A80D4-8931-4D43-ABC0-45ECB90D3687}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F41157F-D7A6-4A52-A65A-DD18118605A0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="881" firstSheet="4" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="881" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Draft Value Calculation Tool" sheetId="21" r:id="rId1"/>
@@ -22,7 +22,9 @@
     <sheet name="Data 1-60" sheetId="1" r:id="rId7"/>
     <sheet name="Clustered Data" sheetId="11" r:id="rId8"/>
     <sheet name="Trendline Data" sheetId="18" r:id="rId9"/>
-    <sheet name="Normalizing Trendlines" sheetId="19" r:id="rId10"/>
+    <sheet name="NBA Draft Pick Value Chart" sheetId="23" r:id="rId10"/>
+    <sheet name="NBA vs NFL Draft Value" sheetId="24" r:id="rId11"/>
+    <sheet name="Normalizing Trendlines" sheetId="19" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="83">
   <si>
     <t>Draft Position</t>
   </si>
@@ -448,6 +450,12 @@
   </si>
   <si>
     <t>WS/ NFL Val</t>
+  </si>
+  <si>
+    <t>NFL</t>
+  </si>
+  <si>
+    <t>NBA</t>
   </si>
 </sst>
 </file>
@@ -8921,6 +8929,1829 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Normalizing Trendlines'!$AF$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NBA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Normalizing Trendlines'!$AE$2:$AE$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Normalizing Trendlines'!$AF$2:$AF$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>2999.9999153764506</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2802.7813416712033</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2618.5278236031163</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2446.3870445545581</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2285.5627187987006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2135.3109080552981</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1994.9365801943325</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1863.7903941688639</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1741.2656963048644</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1626.7957140535389</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1519.8509342250404</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1419.936653575857</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1326.5906904194237</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1239.3812466743736</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1157.9049104607177</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1081.784790004411</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1010.6687702181475</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>944.22788389370646</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>882.15478997134448</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>824.16235184703567</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>769.98230914112162</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>719.36403678426086</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>672.07338568047953</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>627.89159958448613</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>586.61430318295606</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>548.05055669887554</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>512.02197264574716</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>478.36189064595482</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>446.91460649618091</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>417.534651913696</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>390.08612163178668</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>364.44204473161147</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>340.48379730240339</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>318.10055371311137</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>297.18877395718522</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>277.65172469907134</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>259.39903180688458</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>242.34626230137064</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>226.41453378734616</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>211.53014956093006</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>197.62425770465327</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>184.63253259349466</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>172.49487733855864</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>161.15514579196523</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>150.56088282700628</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>140.66308169216225</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>131.41595731654979</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>122.77673451816266</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>114.70545013520245</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>107.16476816520171</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>100.11980705681363</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>93.537978355357936</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>87.388835955731892</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>81.643935265363496</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>76.276701625725877</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>71.262307383758454</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>66.577557044555135</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>62.200779974060026</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58.111730155437385</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>54.291492535410192</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C635-4BA2-B00B-94B7F4A69260}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="488206760"/>
+        <c:axId val="488206432"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="488206760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488206432"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="488206432"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="488206760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>NBA vs NFL Draft</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Value</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Normalizing Trendlines'!$AF$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NBA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Normalizing Trendlines'!$AE$2:$AE$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Normalizing Trendlines'!$AF$2:$AF$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>2999.9999153764506</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2802.7813416712033</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2618.5278236031163</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2446.3870445545581</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2285.5627187987006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2135.3109080552981</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1994.9365801943325</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1863.7903941688639</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1741.2656963048644</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1626.7957140535389</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1519.8509342250404</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1419.936653575857</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1326.5906904194237</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1239.3812466743736</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1157.9049104607177</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1081.784790004411</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1010.6687702181475</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>944.22788389370646</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>882.15478997134448</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>824.16235184703567</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>769.98230914112162</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>719.36403678426086</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>672.07338568047953</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>627.89159958448613</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>586.61430318295606</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>548.05055669887554</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>512.02197264574716</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>478.36189064595482</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>446.91460649618091</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>417.534651913696</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>390.08612163178668</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>364.44204473161147</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>340.48379730240339</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>318.10055371311137</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>297.18877395718522</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>277.65172469907134</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>259.39903180688458</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>242.34626230137064</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>226.41453378734616</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>211.53014956093006</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>197.62425770465327</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>184.63253259349466</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>172.49487733855864</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>161.15514579196523</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>150.56088282700628</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>140.66308169216225</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>131.41595731654979</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>122.77673451816266</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>114.70545013520245</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>107.16476816520171</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>100.11980705681363</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>93.537978355357936</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>87.388835955731892</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>81.643935265363496</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>76.276701625725877</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>71.262307383758454</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>66.577557044555135</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>62.200779974060026</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>58.111730155437385</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>54.291492535410192</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-43FC-4E96-8C39-6B7E9DF0EE76}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Normalizing Trendlines'!$AG$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>NFL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Normalizing Trendlines'!$AE$2:$AE$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>54</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>55</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>59</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Normalizing Trendlines'!$AG$2:$AG$61</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>3000</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2600</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2200</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1800</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1700</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1500</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1400</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1350</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1300</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1250</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1200</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1150</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1100</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1050</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>950</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>875</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>780</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>760</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>740</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>720</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>680</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>660</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>640</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>620</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>580</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>560</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>550</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>540</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>520</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>510</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>490</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>480</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>470</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>460</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>450</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>440</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>420</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>410</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>390</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>380</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>370</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>360</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>350</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>340</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>330</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>320</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>310</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-43FC-4E96-8C39-6B7E9DF0EE76}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="636024200"/>
+        <c:axId val="636025512"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="636024200"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Draft Position</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="636025512"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="636025512"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="3000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Value</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="636024200"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -9082,6 +10913,86 @@
 </file>
 
 <file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -11701,6 +13612,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{6AAB546C-3D3D-4D8A-8F2E-7C7232E0B084}">
   <sheetPr/>
@@ -11750,6 +14693,28 @@
   <sheetPr/>
   <sheetViews>
     <sheetView zoomScale="115" workbookViewId="0"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{F9026E7F-5DEA-493D-B4AD-96B6ADDEB78B}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="50" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{158F2602-6148-4B82-97FE-106972E3ED78}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -12324,6 +15289,72 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8656674" cy="6282070"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B1F81959-18D0-4F49-AC67-0E9FEC1DCC73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8641080" cy="6263640"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59C35F0C-AD1B-4BF9-B412-D95CBC044A81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -21787,15 +24818,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DD0B98-DC49-4BFE-8FC0-1A29CBB95623}">
-  <dimension ref="A1:AB61"/>
+  <dimension ref="A1:AG61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" workbookViewId="0">
-      <selection activeCell="V23" sqref="V23"/>
+    <sheetView topLeftCell="Q1" zoomScale="59" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -21874,8 +24905,17 @@
       <c r="AB1" t="s">
         <v>33</v>
       </c>
+      <c r="AE1" t="s">
+        <v>57</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>82</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -21977,8 +25017,17 @@
         <f t="shared" si="0"/>
         <v>2999.9999879109214</v>
       </c>
+      <c r="AE2">
+        <v>1</v>
+      </c>
+      <c r="AF2">
+        <v>2999.9999153764506</v>
+      </c>
+      <c r="AG2">
+        <v>3000</v>
+      </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -22049,11 +25098,11 @@
         <v>2</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U61" si="16">K3*3000</f>
+        <f t="shared" ref="U3:U59" si="16">K3*3000</f>
         <v>2872.2424587871715</v>
       </c>
       <c r="V3">
-        <f t="shared" ref="V3:V61" si="17">L3*3000</f>
+        <f t="shared" ref="V3:V59" si="17">L3*3000</f>
         <v>2488.8133981550031</v>
       </c>
       <c r="W3">
@@ -22080,8 +25129,17 @@
         <f t="shared" ref="AB3:AB61" si="23">R3*3000</f>
         <v>2708.4859844383263</v>
       </c>
+      <c r="AE3">
+        <v>2</v>
+      </c>
+      <c r="AF3">
+        <v>2802.7813416712033</v>
+      </c>
+      <c r="AG3">
+        <v>2600</v>
+      </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -22183,8 +25241,17 @@
         <f t="shared" si="23"/>
         <v>2509.5607728377813</v>
       </c>
+      <c r="AE4">
+        <v>3</v>
+      </c>
+      <c r="AF4">
+        <v>2618.5278236031163</v>
+      </c>
+      <c r="AG4">
+        <v>2200</v>
+      </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -22286,8 +25353,17 @@
         <f t="shared" si="23"/>
         <v>2350.399109387924</v>
       </c>
+      <c r="AE5">
+        <v>4</v>
+      </c>
+      <c r="AF5">
+        <v>2446.3870445545581</v>
+      </c>
+      <c r="AG5">
+        <v>1800</v>
+      </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -22389,8 +25465,17 @@
         <f t="shared" si="23"/>
         <v>2214.3496777266528</v>
       </c>
+      <c r="AE6">
+        <v>5</v>
+      </c>
+      <c r="AF6">
+        <v>2285.5627187987006</v>
+      </c>
+      <c r="AG6">
+        <v>1700</v>
+      </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -22492,8 +25577,17 @@
         <f t="shared" si="23"/>
         <v>2093.923080644005</v>
       </c>
+      <c r="AE7">
+        <v>6</v>
+      </c>
+      <c r="AF7">
+        <v>2135.3109080552981</v>
+      </c>
+      <c r="AG7">
+        <v>1600</v>
+      </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -22595,8 +25689,17 @@
         <f t="shared" si="23"/>
         <v>1985.0674708972142</v>
       </c>
+      <c r="AE8">
+        <v>7</v>
+      </c>
+      <c r="AF8">
+        <v>1994.9365801943325</v>
+      </c>
+      <c r="AG8">
+        <v>1500</v>
+      </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -22698,8 +25801,17 @@
         <f t="shared" si="23"/>
         <v>1885.3185142200159</v>
       </c>
+      <c r="AE9">
+        <v>8</v>
+      </c>
+      <c r="AF9">
+        <v>1863.7903941688639</v>
+      </c>
+      <c r="AG9">
+        <v>1400</v>
+      </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -22801,8 +25913,17 @@
         <f t="shared" si="23"/>
         <v>1793.049048418306</v>
       </c>
+      <c r="AE10">
+        <v>9</v>
+      </c>
+      <c r="AF10">
+        <v>1741.2656963048644</v>
+      </c>
+      <c r="AG10">
+        <v>1350</v>
+      </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -22904,8 +26025,17 @@
         <f t="shared" si="23"/>
         <v>1707.1166275275255</v>
       </c>
+      <c r="AE11">
+        <v>10</v>
+      </c>
+      <c r="AF11">
+        <v>1626.7957140535389</v>
+      </c>
+      <c r="AG11">
+        <v>1300</v>
+      </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -23007,8 +26137,17 @@
         <f t="shared" si="23"/>
         <v>1626.6797854213448</v>
       </c>
+      <c r="AE12">
+        <v>11</v>
+      </c>
+      <c r="AF12">
+        <v>1519.8509342250404</v>
+      </c>
+      <c r="AG12">
+        <v>1250</v>
+      </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -23110,8 +26249,17 @@
         <f t="shared" si="23"/>
         <v>1551.094446739053</v>
       </c>
+      <c r="AE13">
+        <v>12</v>
+      </c>
+      <c r="AF13">
+        <v>1419.936653575857</v>
+      </c>
+      <c r="AG13">
+        <v>1200</v>
+      </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -23213,8 +26361,17 @@
         <f t="shared" si="23"/>
         <v>1479.8518268272328</v>
       </c>
+      <c r="AE14">
+        <v>13</v>
+      </c>
+      <c r="AF14">
+        <v>1326.5906904194237</v>
+      </c>
+      <c r="AG14">
+        <v>1150</v>
+      </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -23316,8 +26473,17 @@
         <f t="shared" si="23"/>
         <v>1412.5393111259955</v>
       </c>
+      <c r="AE15">
+        <v>14</v>
+      </c>
+      <c r="AF15">
+        <v>1239.3812466743736</v>
+      </c>
+      <c r="AG15">
+        <v>1100</v>
+      </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -23419,8 +26585,17 @@
         <f t="shared" si="23"/>
         <v>1348.8147784692519</v>
       </c>
+      <c r="AE16">
+        <v>15</v>
+      </c>
+      <c r="AF16">
+        <v>1157.9049104607177</v>
+      </c>
+      <c r="AG16">
+        <v>1050</v>
+      </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -23522,8 +26697,17 @@
         <f t="shared" si="23"/>
         <v>1288.3891545982133</v>
       </c>
+      <c r="AE17">
+        <v>16</v>
+      </c>
+      <c r="AF17">
+        <v>1081.784790004411</v>
+      </c>
+      <c r="AG17">
+        <v>1000</v>
+      </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -23625,8 +26809,17 @@
         <f t="shared" si="23"/>
         <v>1231.0142006758333</v>
       </c>
+      <c r="AE18">
+        <v>17</v>
+      </c>
+      <c r="AF18">
+        <v>1010.6687702181475</v>
+      </c>
+      <c r="AG18">
+        <v>950</v>
+      </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -23728,8 +26921,17 @@
         <f t="shared" si="23"/>
         <v>1176.473742609078</v>
       </c>
+      <c r="AE19">
+        <v>18</v>
+      </c>
+      <c r="AF19">
+        <v>944.22788389370646</v>
+      </c>
+      <c r="AG19">
+        <v>900</v>
+      </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -23831,8 +27033,17 @@
         <f t="shared" si="23"/>
         <v>1124.5772271775379</v>
       </c>
+      <c r="AE20">
+        <v>19</v>
+      </c>
+      <c r="AF20">
+        <v>882.15478997134448</v>
+      </c>
+      <c r="AG20">
+        <v>875</v>
+      </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -23934,8 +27145,17 @@
         <f t="shared" si="23"/>
         <v>1075.1548914203411</v>
       </c>
+      <c r="AE21">
+        <v>20</v>
+      </c>
+      <c r="AF21">
+        <v>824.16235184703567</v>
+      </c>
+      <c r="AG21">
+        <v>850</v>
+      </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -24037,8 +27257,17 @@
         <f t="shared" si="23"/>
         <v>1028.0540755804468</v>
       </c>
+      <c r="AE22">
+        <v>21</v>
+      </c>
+      <c r="AF22">
+        <v>769.98230914112162</v>
+      </c>
+      <c r="AG22">
+        <v>800</v>
+      </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -24140,8 +27369,17 @@
         <f t="shared" si="23"/>
         <v>983.13636285428515</v>
       </c>
+      <c r="AE23">
+        <v>22</v>
+      </c>
+      <c r="AF23">
+        <v>719.36403678426086</v>
+      </c>
+      <c r="AG23">
+        <v>780</v>
+      </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -24243,8 +27481,17 @@
         <f t="shared" si="23"/>
         <v>940.27532767987725</v>
       </c>
+      <c r="AE24">
+        <v>23</v>
+      </c>
+      <c r="AF24">
+        <v>672.07338568047953</v>
+      </c>
+      <c r="AG24">
+        <v>760</v>
+      </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -24346,8 +27593,17 @@
         <f t="shared" si="23"/>
         <v>899.35473921494315</v>
       </c>
+      <c r="AE25">
+        <v>24</v>
+      </c>
+      <c r="AF25">
+        <v>627.89159958448613</v>
+      </c>
+      <c r="AG25">
+        <v>740</v>
+      </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -24449,8 +27705,17 @@
         <f t="shared" si="23"/>
         <v>860.26711035897472</v>
       </c>
+      <c r="AE26">
+        <v>25</v>
+      </c>
+      <c r="AF26">
+        <v>586.61430318295606</v>
+      </c>
+      <c r="AG26">
+        <v>720</v>
+      </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -24552,8 +27817,17 @@
         <f t="shared" si="23"/>
         <v>822.91251265865696</v>
       </c>
+      <c r="AE27">
+        <v>26</v>
+      </c>
+      <c r="AF27">
+        <v>548.05055669887554</v>
+      </c>
+      <c r="AG27">
+        <v>700</v>
+      </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -24655,8 +27929,17 @@
         <f t="shared" si="23"/>
         <v>787.19759836880985</v>
       </c>
+      <c r="AE28">
+        <v>27</v>
+      </c>
+      <c r="AF28">
+        <v>512.02197264574716</v>
+      </c>
+      <c r="AG28">
+        <v>680</v>
+      </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -24758,8 +28041,17 @@
         <f t="shared" si="23"/>
         <v>753.0347857870355</v>
       </c>
+      <c r="AE29">
+        <v>28</v>
+      </c>
+      <c r="AF29">
+        <v>478.36189064595482</v>
+      </c>
+      <c r="AG29">
+        <v>660</v>
+      </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -24861,8 +28153,17 @@
         <f t="shared" si="23"/>
         <v>720.34157466330839</v>
       </c>
+      <c r="AE30">
+        <v>29</v>
+      </c>
+      <c r="AF30">
+        <v>446.91460649618091</v>
+      </c>
+      <c r="AG30">
+        <v>640</v>
+      </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -24964,8 +28265,17 @@
         <f t="shared" si="23"/>
         <v>689.03996627663844</v>
       </c>
+      <c r="AE31">
+        <v>30</v>
+      </c>
+      <c r="AF31">
+        <v>417.534651913696</v>
+      </c>
+      <c r="AG31">
+        <v>620</v>
+      </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -25067,8 +28377,17 @@
         <f t="shared" si="23"/>
         <v>659.05596852349402</v>
       </c>
+      <c r="AE32">
+        <v>31</v>
+      </c>
+      <c r="AF32">
+        <v>390.08612163178668</v>
+      </c>
+      <c r="AG32">
+        <v>600</v>
+      </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -25170,8 +28489,17 @@
         <f t="shared" si="23"/>
         <v>630.31917065926962</v>
       </c>
+      <c r="AE33">
+        <v>32</v>
+      </c>
+      <c r="AF33">
+        <v>364.44204473161147</v>
+      </c>
+      <c r="AG33">
+        <v>590</v>
+      </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -25273,8 +28601,17 @@
         <f t="shared" si="23"/>
         <v>602.76237557786828</v>
       </c>
+      <c r="AE34">
+        <v>33</v>
+      </c>
+      <c r="AF34">
+        <v>340.48379730240339</v>
+      </c>
+      <c r="AG34">
+        <v>580</v>
+      </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -25376,8 +28713,17 @@
         <f t="shared" si="23"/>
         <v>576.32127998806891</v>
       </c>
+      <c r="AE35">
+        <v>34</v>
+      </c>
+      <c r="AF35">
+        <v>318.10055371311137</v>
+      </c>
+      <c r="AG35">
+        <v>560</v>
+      </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -25479,8 +28825,17 @@
         <f t="shared" si="23"/>
         <v>550.93419474951133</v>
       </c>
+      <c r="AE36">
+        <v>35</v>
+      </c>
+      <c r="AF36">
+        <v>297.18877395718522</v>
+      </c>
+      <c r="AG36">
+        <v>550</v>
+      </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -25582,8 +28937,17 @@
         <f t="shared" si="23"/>
         <v>526.54179910995708</v>
       </c>
+      <c r="AE37">
+        <v>36</v>
+      </c>
+      <c r="AF37">
+        <v>277.65172469907134</v>
+      </c>
+      <c r="AG37">
+        <v>540</v>
+      </c>
     </row>
-    <row r="38" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -25685,8 +29049,17 @@
         <f t="shared" si="23"/>
         <v>503.08692374365233</v>
       </c>
+      <c r="AE38">
+        <v>37</v>
+      </c>
+      <c r="AF38">
+        <v>259.39903180688458</v>
+      </c>
+      <c r="AG38">
+        <v>530</v>
+      </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -25788,8 +29161,17 @@
         <f t="shared" si="23"/>
         <v>480.51435840483998</v>
       </c>
+      <c r="AE39">
+        <v>38</v>
+      </c>
+      <c r="AF39">
+        <v>242.34626230137064</v>
+      </c>
+      <c r="AG39">
+        <v>520</v>
+      </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -25891,8 +29273,17 @@
         <f t="shared" si="23"/>
         <v>458.77068073758414</v>
       </c>
+      <c r="AE40">
+        <v>39</v>
+      </c>
+      <c r="AF40">
+        <v>226.41453378734616</v>
+      </c>
+      <c r="AG40">
+        <v>510</v>
+      </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -25994,8 +29385,17 @@
         <f t="shared" si="23"/>
         <v>437.80410336549306</v>
       </c>
+      <c r="AE41">
+        <v>40</v>
+      </c>
+      <c r="AF41">
+        <v>211.53014956093006</v>
+      </c>
+      <c r="AG41">
+        <v>500</v>
+      </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -26097,8 +29497,17 @@
         <f t="shared" si="23"/>
         <v>417.56433685464418</v>
       </c>
+      <c r="AE42">
+        <v>41</v>
+      </c>
+      <c r="AF42">
+        <v>197.62425770465327</v>
+      </c>
+      <c r="AG42">
+        <v>490</v>
+      </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -26200,8 +29609,17 @@
         <f t="shared" si="23"/>
         <v>398.00246652430337</v>
       </c>
+      <c r="AE43">
+        <v>42</v>
+      </c>
+      <c r="AF43">
+        <v>184.63253259349466</v>
+      </c>
+      <c r="AG43">
+        <v>480</v>
+      </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -26303,8 +29721,17 @@
         <f t="shared" si="23"/>
         <v>379.07084139144564</v>
       </c>
+      <c r="AE44">
+        <v>43</v>
+      </c>
+      <c r="AF44">
+        <v>172.49487733855864</v>
+      </c>
+      <c r="AG44">
+        <v>470</v>
+      </c>
     </row>
-    <row r="45" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -26406,8 +29833,17 @@
         <f t="shared" si="23"/>
         <v>360.7229737909625</v>
       </c>
+      <c r="AE45">
+        <v>44</v>
+      </c>
+      <c r="AF45">
+        <v>161.15514579196523</v>
+      </c>
+      <c r="AG45">
+        <v>460</v>
+      </c>
     </row>
-    <row r="46" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -26509,8 +29945,17 @@
         <f t="shared" si="23"/>
         <v>342.91344842487513</v>
       </c>
+      <c r="AE46">
+        <v>45</v>
+      </c>
+      <c r="AF46">
+        <v>150.56088282700628</v>
+      </c>
+      <c r="AG46">
+        <v>450</v>
+      </c>
     </row>
-    <row r="47" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -26612,8 +30057,17 @@
         <f t="shared" si="23"/>
         <v>325.59783976954532</v>
       </c>
+      <c r="AE47">
+        <v>46</v>
+      </c>
+      <c r="AF47">
+        <v>140.66308169216225</v>
+      </c>
+      <c r="AG47">
+        <v>440</v>
+      </c>
     </row>
-    <row r="48" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
@@ -26715,8 +30169,17 @@
         <f t="shared" si="23"/>
         <v>308.73263691658582</v>
       </c>
+      <c r="AE48">
+        <v>47</v>
+      </c>
+      <c r="AF48">
+        <v>131.41595731654979</v>
+      </c>
+      <c r="AG48">
+        <v>430</v>
+      </c>
     </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
@@ -26818,8 +30281,17 @@
         <f t="shared" si="23"/>
         <v>292.27517504633704</v>
       </c>
+      <c r="AE49">
+        <v>48</v>
+      </c>
+      <c r="AF49">
+        <v>122.77673451816266</v>
+      </c>
+      <c r="AG49">
+        <v>420</v>
+      </c>
     </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
@@ -26921,8 +30393,17 @@
         <f t="shared" si="23"/>
         <v>276.18357283666455</v>
       </c>
+      <c r="AE50">
+        <v>49</v>
+      </c>
+      <c r="AF50">
+        <v>114.70545013520245</v>
+      </c>
+      <c r="AG50">
+        <v>410</v>
+      </c>
     </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -27024,8 +30505,17 @@
         <f t="shared" si="23"/>
         <v>260.41667519785074</v>
       </c>
+      <c r="AE51">
+        <v>50</v>
+      </c>
+      <c r="AF51">
+        <v>107.16476816520171</v>
+      </c>
+      <c r="AG51">
+        <v>400</v>
+      </c>
     </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -27127,8 +30617,17 @@
         <f t="shared" si="23"/>
         <v>244.93400079930419</v>
       </c>
+      <c r="AE52">
+        <v>51</v>
+      </c>
+      <c r="AF52">
+        <v>100.11980705681363</v>
+      </c>
+      <c r="AG52">
+        <v>390</v>
+      </c>
     </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
@@ -27230,8 +30729,17 @@
         <f t="shared" si="23"/>
         <v>229.69569391786837</v>
       </c>
+      <c r="AE53">
+        <v>52</v>
+      </c>
+      <c r="AF53">
+        <v>93.537978355357936</v>
+      </c>
+      <c r="AG53">
+        <v>380</v>
+      </c>
     </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
@@ -27333,8 +30841,17 @@
         <f t="shared" si="23"/>
         <v>214.66248019249625</v>
       </c>
+      <c r="AE54">
+        <v>53</v>
+      </c>
+      <c r="AF54">
+        <v>87.388835955731892</v>
+      </c>
+      <c r="AG54">
+        <v>370</v>
+      </c>
     </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
@@ -27436,8 +30953,17 @@
         <f t="shared" si="23"/>
         <v>199.79562591746947</v>
       </c>
+      <c r="AE55">
+        <v>54</v>
+      </c>
+      <c r="AF55">
+        <v>81.643935265363496</v>
+      </c>
+      <c r="AG55">
+        <v>360</v>
+      </c>
     </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -27539,8 +31065,17 @@
         <f t="shared" si="23"/>
         <v>185.05690054733802</v>
       </c>
+      <c r="AE56">
+        <v>55</v>
+      </c>
+      <c r="AF56">
+        <v>76.276701625725877</v>
+      </c>
+      <c r="AG56">
+        <v>350</v>
+      </c>
     </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
@@ -27642,8 +31177,17 @@
         <f t="shared" si="23"/>
         <v>170.40854212236206</v>
       </c>
+      <c r="AE57">
+        <v>56</v>
+      </c>
+      <c r="AF57">
+        <v>71.262307383758454</v>
+      </c>
+      <c r="AG57">
+        <v>340</v>
+      </c>
     </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
@@ -27745,8 +31289,17 @@
         <f t="shared" si="23"/>
         <v>155.81322535427253</v>
       </c>
+      <c r="AE58">
+        <v>57</v>
+      </c>
+      <c r="AF58">
+        <v>66.577557044555135</v>
+      </c>
+      <c r="AG58">
+        <v>330</v>
+      </c>
     </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -27848,8 +31401,17 @@
         <f t="shared" si="23"/>
         <v>141.23403213929564</v>
       </c>
+      <c r="AE59">
+        <v>58</v>
+      </c>
+      <c r="AF59">
+        <v>62.200779974060026</v>
+      </c>
+      <c r="AG59">
+        <v>320</v>
+      </c>
     </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -27949,8 +31511,17 @@
         <f t="shared" si="23"/>
         <v>126.63442428917909</v>
       </c>
+      <c r="AE60">
+        <v>59</v>
+      </c>
+      <c r="AF60">
+        <v>58.111730155437385</v>
+      </c>
+      <c r="AG60">
+        <v>310</v>
+      </c>
     </row>
-    <row r="61" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -28049,6 +31620,15 @@
       <c r="AB61">
         <f t="shared" si="23"/>
         <v>111.97821829191645</v>
+      </c>
+      <c r="AE61">
+        <v>60</v>
+      </c>
+      <c r="AF61">
+        <v>54.291492535410192</v>
+      </c>
+      <c r="AG61">
+        <v>300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to report ready for branch
</commit_message>
<xml_diff>
--- a/Plot/Final_Draft_Position_Graphs.xlsx
+++ b/Plot/Final_Draft_Position_Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Desktop\MQP\Plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F41157F-D7A6-4A52-A65A-DD18118605A0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210B71FF-564A-4088-A36E-0233FE90A736}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="881" firstSheet="10" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8412" yWindow="816" windowWidth="23256" windowHeight="13176" tabRatio="881" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Draft Value Calculation Tool" sheetId="21" r:id="rId1"/>
@@ -14714,7 +14714,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{158F2602-6148-4B82-97FE-106972E3ED78}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="86" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -15326,7 +15326,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8641080" cy="6263640"/>
+    <xdr:ext cx="8656674" cy="6282070"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -24820,8 +24820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DD0B98-DC49-4BFE-8FC0-1A29CBB95623}">
   <dimension ref="A1:AG61"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" zoomScale="59" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2"/>
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="96" workbookViewId="0">
+      <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
first draft of report!
</commit_message>
<xml_diff>
--- a/Plot/Final_Draft_Position_Graphs.xlsx
+++ b/Plot/Final_Draft_Position_Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Desktop\MQP\Plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{210B71FF-564A-4088-A36E-0233FE90A736}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2544D818-82B6-466C-AEF9-8BBE1BF0403E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8412" yWindow="816" windowWidth="23256" windowHeight="13176" tabRatio="881" firstSheet="5" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960" tabRatio="881" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Draft Value Calculation Tool" sheetId="21" r:id="rId1"/>
@@ -14681,7 +14681,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{12FFEA56-D690-4F65-A8CE-5A70D0B0245D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -14791,7 +14791,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8654815" cy="6274741"/>
+    <xdr:ext cx="8659906" cy="6284259"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -24820,7 +24820,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72DD0B98-DC49-4BFE-8FC0-1A29CBB95623}">
   <dimension ref="A1:AG61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="96" workbookViewId="0">
+    <sheetView topLeftCell="X1" zoomScale="96" workbookViewId="0">
       <selection activeCell="AH1" sqref="AH1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed color schemes, added text
</commit_message>
<xml_diff>
--- a/Plot/Final_Draft_Position_Graphs.xlsx
+++ b/Plot/Final_Draft_Position_Graphs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jake\Desktop\MQP\Plot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2544D818-82B6-466C-AEF9-8BBE1BF0403E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DD633B-42B1-4923-A3B7-AB39B8AEE75B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960" tabRatio="881" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12960" tabRatio="881" firstSheet="4" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Draft Value Calculation Tool" sheetId="21" r:id="rId1"/>
@@ -6577,7 +6577,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -6988,7 +6988,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -7399,7 +7399,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:srgbClr val="7030A0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -7810,7 +7810,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent5"/>
+                <a:srgbClr val="0070C0"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -8221,7 +8221,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent6"/>
+                <a:srgbClr val="FFC000"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -14681,7 +14681,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{12FFEA56-D690-4F65-A8CE-5A70D0B0245D}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" workbookViewId="0"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -15260,7 +15260,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8656674" cy="6282070"/>
+    <xdr:ext cx="8660296" cy="6281530"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">

</xml_diff>